<commit_message>
trainModel updated! mockTrade completed!
</commit_message>
<xml_diff>
--- a/Original/Files/计算比例.xlsx
+++ b/Original/Files/计算比例.xlsx
@@ -243,7 +243,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -261,6 +261,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -584,15 +585,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E20" sqref="A14:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" customWidth="1"/>
+    <col min="1" max="1" width="8.25" customWidth="1"/>
     <col min="2" max="2" width="10.375" customWidth="1"/>
     <col min="3" max="4" width="9.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.75" customWidth="1"/>
@@ -766,6 +767,9 @@
     </row>
     <row r="13" spans="1:5">
       <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>